<commit_message>
Add 2026 to map filter options.
</commit_message>
<xml_diff>
--- a/States_FIPS.xlsx
+++ b/States_FIPS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://txriogrande-my.sharepoint.com/personal/eshackney_trla_org/Documents/Projects/Active/Farmworker Data Project/Farmworker Frontend Shiny/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://txriogrande-my.sharepoint.com/personal/anovak_trla_org/Documents/Farmworker Projects/trla-H2Data-frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{3F9E55AC-3A7B-4AB9-8F6F-F512ED5210D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC6FB670-6592-44C7-B50B-58E9449B6E2E}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{3F9E55AC-3A7B-4AB9-8F6F-F512ED5210D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFFA2B25-CAC1-464E-B0C3-C051C35BFA6A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="States_FIPS" sheetId="1" r:id="rId1"/>
@@ -928,9 +928,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -968,7 +968,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1074,7 +1074,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1216,7 +1216,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1227,11 +1227,12 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="23.81640625" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>